<commit_message>
Fix translation col order in the last commit
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_latrine/forms/hh_latrine/hh_latrine.xlsx
+++ b/odkx/app/config/tables/hh_latrine/forms/hh_latrine/hh_latrine.xlsx
@@ -267,13 +267,13 @@
     <t xml:space="preserve">41c (iii). Na kaya ngapi? (bila kujumuisha kaya hii</t>
   </si>
   <si>
-    <t xml:space="preserve">Household Identification {{data.hh_id}}</t>
+    <t xml:space="preserve">Household ID: {{data.hh_id}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificação do agregado{{data.hh_id}}</t>
   </si>
   <si>
     <t xml:space="preserve">Utambulisho wa Kaya {{data.hh_id}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identificação do agregado{{data.hh_id}}</t>
   </si>
   <si>
     <t xml:space="preserve">Toilet connected to septic tank</t>
@@ -543,7 +543,7 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1588,7 +1588,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1731,7 +1731,7 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1869,7 +1869,7 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3009,7 +3009,7 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4083,8 +4083,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4290,7 +4290,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576 C1:D4 C6:D1048576">
+  <conditionalFormatting sqref="B1:D4 B6:D1048576 B5">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>